<commit_message>
fix row number sorting to work for multi digit numbers
</commit_message>
<xml_diff>
--- a/spec/support/static_test_files/as_tables.xlsx
+++ b/spec/support/static_test_files/as_tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/f3m-mbp1/dev/f3mmedia/rxl/spec/support/static_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B678147-2666-1042-9E38-BE530E48FBC4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7AC7A6-89A1-8B4B-9338-532641E2D8D2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31160" yWindow="2660" windowWidth="25640" windowHeight="13000" activeTab="1" xr2:uid="{5EB412A2-8117-E244-B1FD-60CE04426CE9}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>header_1</t>
   </si>
@@ -64,28 +64,40 @@
     <t>sum_3</t>
   </si>
   <si>
-    <t>header_4</t>
-  </si>
-  <si>
-    <t>row_1_d</t>
-  </si>
-  <si>
-    <t>row_2_d</t>
-  </si>
-  <si>
-    <t>sum_4</t>
-  </si>
-  <si>
     <t>row_3_a</t>
   </si>
   <si>
     <t>row_3_b</t>
   </si>
   <si>
-    <t>row_3_c</t>
-  </si>
-  <si>
-    <t>row_3_d</t>
+    <t>row_4_a</t>
+  </si>
+  <si>
+    <t>row_5_a</t>
+  </si>
+  <si>
+    <t>row_5_b</t>
+  </si>
+  <si>
+    <t>row_6_a</t>
+  </si>
+  <si>
+    <t>row_6_b</t>
+  </si>
+  <si>
+    <t>row_7_a</t>
+  </si>
+  <si>
+    <t>row_7_b</t>
+  </si>
+  <si>
+    <t>row_8_a</t>
+  </si>
+  <si>
+    <t>row_8_b</t>
+  </si>
+  <si>
+    <t>row_4_b</t>
   </si>
 </sst>
 </file>
@@ -496,82 +508,92 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE8E26A5-026F-2949-B32F-EAF096239E02}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="D4" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B12" t="s">
         <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>